<commit_message>
Outcomes: games through 1-12-25
</commit_message>
<xml_diff>
--- a/ncaaModelOutcomes.xlsx
+++ b/ncaaModelOutcomes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/isaiahnick/Desktop/NCAAM/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0927CE54-9C4C-9645-B2CD-CA15BDEE32B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D46319E-B535-DE48-8807-AD4AFE0FFDFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="39940" yWindow="3160" windowWidth="28220" windowHeight="16380" xr2:uid="{48E97E4C-EE8F-4D4C-B07B-683BDA3BBCA7}"/>
+    <workbookView xWindow="39940" yWindow="3160" windowWidth="28220" windowHeight="16380" activeTab="6" xr2:uid="{48E97E4C-EE8F-4D4C-B07B-683BDA3BBCA7}"/>
   </bookViews>
   <sheets>
     <sheet name="Champions" sheetId="2" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="621" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="621" uniqueCount="180">
   <si>
     <t>Team</t>
   </si>
@@ -137,9 +137,6 @@
     <t>Arizona</t>
   </si>
   <si>
-    <t>P12</t>
-  </si>
-  <si>
     <t>Texas A&amp;M</t>
   </si>
   <si>
@@ -152,9 +149,6 @@
     <t>Mississippi St.</t>
   </si>
   <si>
-    <t>St. John's</t>
-  </si>
-  <si>
     <t>Wisconsin</t>
   </si>
   <si>
@@ -170,9 +164,6 @@
     <t>Pittsburgh</t>
   </si>
   <si>
-    <t>Saint Mary's</t>
-  </si>
-  <si>
     <t>Clemson</t>
   </si>
   <si>
@@ -215,9 +206,6 @@
     <t>Creighton</t>
   </si>
   <si>
-    <t>VCU</t>
-  </si>
-  <si>
     <t>A10</t>
   </si>
   <si>
@@ -437,15 +425,9 @@
     <t>BW</t>
   </si>
   <si>
-    <t>UC Irvine</t>
-  </si>
-  <si>
     <t>CUSA</t>
   </si>
   <si>
-    <t>North Texas</t>
-  </si>
-  <si>
     <t>BSth</t>
   </si>
   <si>
@@ -467,9 +449,6 @@
     <t>CAA</t>
   </si>
   <si>
-    <t>George Mason</t>
-  </si>
-  <si>
     <t>ASun</t>
   </si>
   <si>
@@ -497,9 +476,6 @@
     <t>OVC</t>
   </si>
   <si>
-    <t>Murray St.</t>
-  </si>
-  <si>
     <t>Sum</t>
   </si>
   <si>
@@ -518,12 +494,6 @@
     <t>Northern Colorado</t>
   </si>
   <si>
-    <t>GWC</t>
-  </si>
-  <si>
-    <t>Utah Valley</t>
-  </si>
-  <si>
     <t>MEAC</t>
   </si>
   <si>
@@ -533,33 +503,18 @@
     <t>Slnd</t>
   </si>
   <si>
-    <t>Sam Houston St.</t>
-  </si>
-  <si>
     <t>Horz</t>
   </si>
   <si>
-    <t>Illinois Chicago</t>
-  </si>
-  <si>
     <t>AE</t>
   </si>
   <si>
-    <t>UMass Lowell</t>
-  </si>
-  <si>
     <t>NEC</t>
   </si>
   <si>
-    <t>Bryant</t>
-  </si>
-  <si>
     <t>MAAC</t>
   </si>
   <si>
-    <t>Marist</t>
-  </si>
-  <si>
     <t>SWAC</t>
   </si>
   <si>
@@ -575,9 +530,6 @@
     <t>Connecticut</t>
   </si>
   <si>
-    <t>UCLA</t>
-  </si>
-  <si>
     <t>Cincinnati</t>
   </si>
   <si>
@@ -588,6 +540,48 @@
   </si>
   <si>
     <t>Total Teams</t>
+  </si>
+  <si>
+    <t>St. John'S</t>
+  </si>
+  <si>
+    <t>Saint Mary'S</t>
+  </si>
+  <si>
+    <t>Vcu</t>
+  </si>
+  <si>
+    <t>Uc Irvine</t>
+  </si>
+  <si>
+    <t>High Point</t>
+  </si>
+  <si>
+    <t>Charleston</t>
+  </si>
+  <si>
+    <t>Purdue Fort Wayne</t>
+  </si>
+  <si>
+    <t>Texas A&amp;M Corpus Chris</t>
+  </si>
+  <si>
+    <t>Umass Lowell</t>
+  </si>
+  <si>
+    <t>Merrimack</t>
+  </si>
+  <si>
+    <t>Central Connecticut</t>
+  </si>
+  <si>
+    <t>Little Rock</t>
+  </si>
+  <si>
+    <t>Ucla</t>
+  </si>
+  <si>
+    <t>Villanova</t>
   </si>
 </sst>
 </file>
@@ -975,7 +969,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18BC26E8-D6C2-0E4A-830A-7AA78E1502E8}">
   <dimension ref="A1:H32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="106" workbookViewId="0"/>
+    <sheetView zoomScale="106" workbookViewId="0">
+      <selection activeCell="K17" sqref="K17"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -984,43 +980,43 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B1" s="1"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
@@ -1106,7 +1102,7 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C14" s="2">
         <v>0.121</v>
@@ -1314,7 +1310,7 @@
         <v>30</v>
       </c>
       <c r="B22" t="s">
-        <v>31</v>
+        <v>15</v>
       </c>
       <c r="C22" s="2">
         <v>3.3000000000000002E-2</v>
@@ -1337,7 +1333,7 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B23" t="s">
         <v>15</v>
@@ -1363,7 +1359,7 @@
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B24" t="s">
         <v>4</v>
@@ -1389,7 +1385,7 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B25" t="s">
         <v>23</v>
@@ -1415,10 +1411,10 @@
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B26" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="C26" s="2">
         <v>3.0000000000000001E-3</v>
@@ -1441,27 +1437,27 @@
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -1474,7 +1470,7 @@
   <dimension ref="A1:H36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D32" sqref="D32"/>
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1484,42 +1480,42 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
@@ -1605,7 +1601,7 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C14" s="2">
         <v>0.185</v>
@@ -1865,7 +1861,7 @@
         <v>30</v>
       </c>
       <c r="B24" t="s">
-        <v>31</v>
+        <v>15</v>
       </c>
       <c r="C24" s="2">
         <v>6.4000000000000001E-2</v>
@@ -1888,7 +1884,7 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B25" t="s">
         <v>15</v>
@@ -1940,7 +1936,7 @@
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B27" t="s">
         <v>4</v>
@@ -1966,7 +1962,7 @@
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B28" t="s">
         <v>4</v>
@@ -1992,7 +1988,7 @@
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B29" t="s">
         <v>23</v>
@@ -2018,7 +2014,7 @@
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B30" t="s">
         <v>4</v>
@@ -2044,27 +2040,27 @@
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
     </row>
   </sheetData>
@@ -2074,10 +2070,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF812A5C-DFB4-0842-994A-1F991B822E52}">
-  <dimension ref="A1:H46"/>
+  <dimension ref="A1:H47"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M18" sqref="M18"/>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2087,42 +2083,42 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
@@ -2208,7 +2204,7 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C14" s="2">
         <v>0.28100000000000003</v>
@@ -2494,7 +2490,7 @@
         <v>30</v>
       </c>
       <c r="B25" t="s">
-        <v>31</v>
+        <v>15</v>
       </c>
       <c r="C25" s="2">
         <v>0.128</v>
@@ -2543,7 +2539,7 @@
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B27" t="s">
         <v>4</v>
@@ -2569,7 +2565,7 @@
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B28" t="s">
         <v>15</v>
@@ -2595,7 +2591,7 @@
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B29" t="s">
         <v>4</v>
@@ -2621,7 +2617,7 @@
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B30" t="s">
         <v>23</v>
@@ -2647,7 +2643,7 @@
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>36</v>
+        <v>166</v>
       </c>
       <c r="B31" t="s">
         <v>25</v>
@@ -2673,7 +2669,7 @@
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B32" t="s">
         <v>4</v>
@@ -2699,10 +2695,10 @@
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B33" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="C33" s="2">
         <v>7.8E-2</v>
@@ -2725,10 +2721,10 @@
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B34" t="s">
-        <v>25</v>
+        <v>6</v>
       </c>
       <c r="C34" s="2">
         <v>6.3E-2</v>
@@ -2751,7 +2747,7 @@
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>42</v>
+        <v>167</v>
       </c>
       <c r="B35" t="s">
         <v>21</v>
@@ -2777,7 +2773,7 @@
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B36" t="s">
         <v>6</v>
@@ -2803,7 +2799,7 @@
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B37" t="s">
         <v>6</v>
@@ -2829,7 +2825,7 @@
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B38" t="s">
         <v>23</v>
@@ -2855,7 +2851,7 @@
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B39" t="s">
         <v>13</v>
@@ -2881,10 +2877,10 @@
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B40" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="C40" s="2">
         <v>2.7E-2</v>
@@ -2905,29 +2901,29 @@
         <v>1.25</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A42" t="s">
-        <v>68</v>
-      </c>
-    </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>90</v>
+        <v>64</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>71</v>
+        <v>87</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>92</v>
+        <v>67</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>88</v>
       </c>
     </row>
   </sheetData>
@@ -2939,8 +2935,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0825CF93-4158-144F-A7C0-50341FAA3534}">
   <dimension ref="A1:H50"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D57" sqref="D57"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2950,43 +2946,43 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="B1" s="1"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
@@ -3072,7 +3068,7 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C14" s="2">
         <v>0.51</v>
@@ -3410,7 +3406,7 @@
         <v>30</v>
       </c>
       <c r="B27" t="s">
-        <v>31</v>
+        <v>15</v>
       </c>
       <c r="C27" s="2">
         <v>0.23599999999999999</v>
@@ -3433,7 +3429,7 @@
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B28" t="s">
         <v>4</v>
@@ -3459,7 +3455,7 @@
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B29" t="s">
         <v>15</v>
@@ -3485,7 +3481,7 @@
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B30" t="s">
         <v>4</v>
@@ -3511,7 +3507,7 @@
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>36</v>
+        <v>166</v>
       </c>
       <c r="B31" t="s">
         <v>25</v>
@@ -3537,7 +3533,7 @@
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B32" t="s">
         <v>23</v>
@@ -3563,7 +3559,7 @@
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B33" t="s">
         <v>23</v>
@@ -3589,7 +3585,7 @@
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B34" t="s">
         <v>4</v>
@@ -3615,10 +3611,10 @@
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B35" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="C35" s="2">
         <v>0.155</v>
@@ -3641,10 +3637,10 @@
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B36" t="s">
-        <v>25</v>
+        <v>6</v>
       </c>
       <c r="C36" s="2">
         <v>0.126</v>
@@ -3667,7 +3663,7 @@
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>42</v>
+        <v>167</v>
       </c>
       <c r="B37" t="s">
         <v>21</v>
@@ -3693,7 +3689,7 @@
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B38" t="s">
         <v>6</v>
@@ -3719,7 +3715,7 @@
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B39" t="s">
         <v>6</v>
@@ -3745,7 +3741,7 @@
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B40" t="s">
         <v>23</v>
@@ -3771,7 +3767,7 @@
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B41" t="s">
         <v>13</v>
@@ -3797,10 +3793,10 @@
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B42" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="C42" s="2">
         <v>7.3999999999999996E-2</v>
@@ -3823,10 +3819,10 @@
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B43" t="s">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="C43" s="2">
         <v>5.7000000000000002E-2</v>
@@ -3849,7 +3845,7 @@
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B44" t="s">
         <v>4</v>
@@ -3875,27 +3871,27 @@
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
     </row>
   </sheetData>
@@ -3908,7 +3904,7 @@
   <dimension ref="A1:H52"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H39" sqref="H39"/>
+      <selection activeCell="I30" sqref="I30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3918,48 +3914,48 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="B10" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
@@ -3970,10 +3966,10 @@
         <v>1</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="D11" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="E11" t="s">
         <v>2</v>
@@ -4045,7 +4041,7 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C14" s="2">
         <v>0.91100000000000003</v>
@@ -4383,7 +4379,7 @@
         <v>30</v>
       </c>
       <c r="B27" t="s">
-        <v>31</v>
+        <v>15</v>
       </c>
       <c r="C27" s="2">
         <v>0.45800000000000002</v>
@@ -4406,7 +4402,7 @@
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B28" t="s">
         <v>4</v>
@@ -4432,7 +4428,7 @@
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B29" t="s">
         <v>15</v>
@@ -4458,7 +4454,7 @@
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B30" t="s">
         <v>4</v>
@@ -4484,7 +4480,7 @@
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>36</v>
+        <v>166</v>
       </c>
       <c r="B31" t="s">
         <v>25</v>
@@ -4510,7 +4506,7 @@
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B32" t="s">
         <v>23</v>
@@ -4536,7 +4532,7 @@
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B33" t="s">
         <v>23</v>
@@ -4562,7 +4558,7 @@
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B34" t="s">
         <v>4</v>
@@ -4588,10 +4584,10 @@
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B35" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="C35" s="2">
         <v>0.32400000000000001</v>
@@ -4614,10 +4610,10 @@
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B36" t="s">
-        <v>25</v>
+        <v>6</v>
       </c>
       <c r="C36" s="2">
         <v>0.27500000000000002</v>
@@ -4640,7 +4636,7 @@
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>42</v>
+        <v>167</v>
       </c>
       <c r="B37" t="s">
         <v>21</v>
@@ -4666,7 +4662,7 @@
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B38" t="s">
         <v>6</v>
@@ -4692,7 +4688,7 @@
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B39" t="s">
         <v>6</v>
@@ -4718,7 +4714,7 @@
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B40" t="s">
         <v>23</v>
@@ -4744,7 +4740,7 @@
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B41" t="s">
         <v>13</v>
@@ -4770,10 +4766,10 @@
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B42" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="C42" s="2">
         <v>0.19</v>
@@ -4796,10 +4792,10 @@
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B43" t="s">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="C43" s="2">
         <v>0.16200000000000001</v>
@@ -4822,7 +4818,7 @@
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B44" t="s">
         <v>4</v>
@@ -4848,10 +4844,10 @@
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B45" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C45" s="2">
         <v>0.122</v>
@@ -4874,7 +4870,7 @@
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B46" t="s">
         <v>25</v>
@@ -4900,27 +4896,27 @@
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
     </row>
   </sheetData>
@@ -4932,8 +4928,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{645CF770-8328-7447-B6BD-A2D494CAA547}">
   <dimension ref="A1:H58"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K18" sqref="K18"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="K31" sqref="K31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4943,42 +4939,42 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
@@ -5064,7 +5060,7 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C14" s="2">
         <v>0.91500000000000004</v>
@@ -5402,7 +5398,7 @@
         <v>30</v>
       </c>
       <c r="B27" t="s">
-        <v>31</v>
+        <v>15</v>
       </c>
       <c r="C27" s="2">
         <v>0.51300000000000001</v>
@@ -5425,7 +5421,7 @@
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B28" t="s">
         <v>4</v>
@@ -5451,7 +5447,7 @@
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B29" t="s">
         <v>15</v>
@@ -5477,7 +5473,7 @@
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B30" t="s">
         <v>4</v>
@@ -5503,7 +5499,7 @@
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B31" t="s">
         <v>4</v>
@@ -5529,7 +5525,7 @@
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>36</v>
+        <v>166</v>
       </c>
       <c r="B32" t="s">
         <v>25</v>
@@ -5555,7 +5551,7 @@
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B33" t="s">
         <v>23</v>
@@ -5581,7 +5577,7 @@
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B34" t="s">
         <v>23</v>
@@ -5607,7 +5603,7 @@
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B35" t="s">
         <v>4</v>
@@ -5633,10 +5629,10 @@
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B36" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="C36" s="2">
         <v>0.39400000000000002</v>
@@ -5659,10 +5655,10 @@
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B37" t="s">
-        <v>25</v>
+        <v>6</v>
       </c>
       <c r="C37" s="2">
         <v>0.35099999999999998</v>
@@ -5685,7 +5681,7 @@
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>42</v>
+        <v>167</v>
       </c>
       <c r="B38" t="s">
         <v>21</v>
@@ -5711,7 +5707,7 @@
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B39" t="s">
         <v>6</v>
@@ -5737,7 +5733,7 @@
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B40" t="s">
         <v>6</v>
@@ -5763,7 +5759,7 @@
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B41" t="s">
         <v>23</v>
@@ -5789,7 +5785,7 @@
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B42" t="s">
         <v>23</v>
@@ -5815,7 +5811,7 @@
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B43" t="s">
         <v>13</v>
@@ -5841,10 +5837,10 @@
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B44" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="C44" s="2">
         <v>0.27400000000000002</v>
@@ -5867,7 +5863,7 @@
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B45" t="s">
         <v>4</v>
@@ -5893,7 +5889,7 @@
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B46" t="s">
         <v>23</v>
@@ -5919,10 +5915,10 @@
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B47" t="s">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="C47" s="2">
         <v>0.249</v>
@@ -5945,7 +5941,7 @@
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B48" t="s">
         <v>4</v>
@@ -5971,10 +5967,10 @@
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B49" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C49" s="2">
         <v>0.215</v>
@@ -5997,10 +5993,10 @@
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B50" t="s">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="C50" s="2">
         <v>0.21199999999999999</v>
@@ -6023,7 +6019,7 @@
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B51" t="s">
         <v>25</v>
@@ -6049,10 +6045,10 @@
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>57</v>
+        <v>168</v>
       </c>
       <c r="B52" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="C52" s="2">
         <v>0.2</v>
@@ -6075,27 +6071,27 @@
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
     </row>
   </sheetData>
@@ -6107,20 +6103,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A04F142-2826-6D40-AD77-493323D02C9D}">
   <dimension ref="A1:C80"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A47" workbookViewId="0">
+      <selection activeCell="B80" sqref="B80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -6131,7 +6127,7 @@
         <v>0</v>
       </c>
       <c r="C4" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -6158,7 +6154,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B7" t="s">
         <v>12</v>
@@ -6169,57 +6165,57 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="B8" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="C8">
-        <v>31.4</v>
+        <v>26.84</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B9" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C9">
-        <v>26.84</v>
+        <v>26.14</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B10" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C10">
-        <v>26.14</v>
+        <v>25.69</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="B11" t="s">
-        <v>24</v>
+        <v>44</v>
       </c>
       <c r="C11">
-        <v>25.69</v>
+        <v>18.18</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>31</v>
+        <v>51</v>
       </c>
       <c r="B12" t="s">
-        <v>30</v>
+        <v>125</v>
       </c>
       <c r="C12">
-        <v>23.97</v>
+        <v>17.670000000000002</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
@@ -6227,367 +6223,367 @@
         <v>54</v>
       </c>
       <c r="B13" t="s">
-        <v>129</v>
+        <v>168</v>
       </c>
       <c r="C13">
-        <v>17.670000000000002</v>
+        <v>16.190000000000001</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>58</v>
+        <v>126</v>
       </c>
       <c r="B14" t="s">
-        <v>57</v>
+        <v>169</v>
       </c>
       <c r="C14">
-        <v>16.190000000000001</v>
+        <v>13.97</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="B15" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C15">
-        <v>13.97</v>
+        <v>11.46</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B16" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C16">
-        <v>12.63</v>
+        <v>10.79</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B17" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C17">
-        <v>11.46</v>
+        <v>10.16</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
+        <v>135</v>
+      </c>
+      <c r="B18" t="s">
         <v>136</v>
       </c>
-      <c r="B18" t="s">
-        <v>137</v>
-      </c>
       <c r="C18">
-        <v>10.79</v>
+        <v>8.83</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
+        <v>137</v>
+      </c>
+      <c r="B19" t="s">
         <v>138</v>
       </c>
-      <c r="B19" t="s">
-        <v>139</v>
-      </c>
       <c r="C19">
-        <v>10.16</v>
+        <v>7.05</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
+        <v>139</v>
+      </c>
+      <c r="B20" t="s">
         <v>140</v>
       </c>
-      <c r="B20" t="s">
-        <v>141</v>
-      </c>
       <c r="C20">
-        <v>9.0399999999999991</v>
+        <v>6.37</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>142</v>
+        <v>128</v>
       </c>
       <c r="B21" t="s">
-        <v>143</v>
+        <v>170</v>
       </c>
       <c r="C21">
-        <v>8.83</v>
+        <v>6.25</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="B22" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="C22">
-        <v>7.05</v>
+        <v>5.67</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B23" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C23">
-        <v>6.37</v>
+        <v>4.8099999999999996</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B24" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C24">
-        <v>5.67</v>
+        <v>4.12</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>150</v>
+        <v>134</v>
       </c>
       <c r="B25" t="s">
-        <v>151</v>
+        <v>171</v>
       </c>
       <c r="C25">
-        <v>4.9800000000000004</v>
+        <v>2.59</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="B26" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="C26">
-        <v>4.8099999999999996</v>
+        <v>2.46</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B27" t="s">
-        <v>155</v>
+        <v>172</v>
       </c>
       <c r="C27">
-        <v>4.12</v>
+        <v>2.34</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="B28" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="C28">
-        <v>2.46</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="B29" t="s">
-        <v>159</v>
+        <v>173</v>
       </c>
       <c r="C29">
-        <v>1.1200000000000001</v>
+        <v>0.62</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="B30" t="s">
-        <v>161</v>
+        <v>174</v>
       </c>
       <c r="C30">
-        <v>1</v>
+        <v>0.37</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="B31" t="s">
-        <v>163</v>
+        <v>175</v>
       </c>
       <c r="C31">
-        <v>0.98</v>
+        <v>-1.8</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="B32" t="s">
-        <v>165</v>
+        <v>176</v>
       </c>
       <c r="C32">
-        <v>0.92</v>
+        <v>-3.89</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
       <c r="B33" t="s">
-        <v>167</v>
+        <v>158</v>
       </c>
       <c r="C33">
-        <v>0.37</v>
+        <v>-4.9800000000000004</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>168</v>
+        <v>159</v>
       </c>
       <c r="B34" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
       <c r="C34">
-        <v>-0.83</v>
+        <v>-5.82</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>170</v>
+        <v>143</v>
       </c>
       <c r="B35" t="s">
-        <v>171</v>
+        <v>177</v>
       </c>
       <c r="C35">
-        <v>-4.2300000000000004</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
-        <v>172</v>
-      </c>
-      <c r="B36" t="s">
-        <v>173</v>
-      </c>
-      <c r="C36">
-        <v>-4.9800000000000004</v>
+        <v>-6.29</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>174</v>
-      </c>
-      <c r="B37" t="s">
-        <v>175</v>
-      </c>
-      <c r="C37">
-        <v>-5.82</v>
+        <v>122</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>0</v>
+      </c>
+      <c r="B38" t="s">
+        <v>1</v>
+      </c>
+      <c r="C38" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>126</v>
+        <v>14</v>
+      </c>
+      <c r="B39" t="s">
+        <v>15</v>
+      </c>
+      <c r="C39">
+        <v>31.4</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="B40" t="s">
-        <v>1</v>
-      </c>
-      <c r="C40" t="s">
-        <v>128</v>
+        <v>4</v>
+      </c>
+      <c r="C40">
+        <v>30.13</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B41" t="s">
         <v>4</v>
       </c>
       <c r="C41">
-        <v>30.13</v>
+        <v>29.26</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B42" t="s">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="C42">
-        <v>29.26</v>
+        <v>28.33</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B43" t="s">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="C43">
-        <v>28.33</v>
+        <v>27.8</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="B44" t="s">
-        <v>4</v>
+        <v>23</v>
       </c>
       <c r="C44">
-        <v>27.8</v>
+        <v>25.18</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B45" t="s">
         <v>23</v>
       </c>
       <c r="C45">
-        <v>25.18</v>
+        <v>24.39</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B46" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="C46">
-        <v>24.39</v>
+        <v>23.98</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B47" t="s">
         <v>15</v>
       </c>
       <c r="C47">
-        <v>23.98</v>
+        <v>23.97</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.2">
@@ -6603,7 +6599,7 @@
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B49" t="s">
         <v>4</v>
@@ -6614,7 +6610,7 @@
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B50" t="s">
         <v>15</v>
@@ -6625,7 +6621,7 @@
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>36</v>
+        <v>166</v>
       </c>
       <c r="B51" t="s">
         <v>25</v>
@@ -6636,7 +6632,7 @@
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B52" t="s">
         <v>4</v>
@@ -6647,7 +6643,7 @@
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B53" t="s">
         <v>4</v>
@@ -6658,7 +6654,7 @@
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B54" t="s">
         <v>23</v>
@@ -6669,7 +6665,7 @@
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B55" t="s">
         <v>23</v>
@@ -6680,7 +6676,7 @@
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B56" t="s">
         <v>4</v>
@@ -6691,7 +6687,7 @@
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>176</v>
+        <v>161</v>
       </c>
       <c r="B57" t="s">
         <v>25</v>
@@ -6702,10 +6698,10 @@
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B58" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="C58">
         <v>20.97</v>
@@ -6713,10 +6709,10 @@
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B59" t="s">
-        <v>25</v>
+        <v>6</v>
       </c>
       <c r="C59">
         <v>19.850000000000001</v>
@@ -6724,7 +6720,7 @@
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>42</v>
+        <v>167</v>
       </c>
       <c r="B60" t="s">
         <v>21</v>
@@ -6735,7 +6731,7 @@
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B61" t="s">
         <v>6</v>
@@ -6746,7 +6742,7 @@
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B62" t="s">
         <v>6</v>
@@ -6757,10 +6753,10 @@
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B63" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="C63">
         <v>18.98</v>
@@ -6768,7 +6764,7 @@
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B64" t="s">
         <v>23</v>
@@ -6779,7 +6775,7 @@
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B65" t="s">
         <v>23</v>
@@ -6790,138 +6786,138 @@
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B66" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="C66">
-        <v>18.18</v>
+        <v>17.96</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B67" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="C67">
-        <v>17.96</v>
+        <v>17.899999999999999</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B68" t="s">
         <v>4</v>
       </c>
       <c r="C68">
-        <v>17.899999999999999</v>
+        <v>17.329999999999998</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B69" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="C69">
-        <v>17.329999999999998</v>
+        <v>17.25</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>50</v>
+        <v>162</v>
       </c>
       <c r="B70" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="C70">
-        <v>17.25</v>
+        <v>17.170000000000002</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>178</v>
+        <v>49</v>
       </c>
       <c r="B71" t="s">
-        <v>25</v>
+        <v>4</v>
       </c>
       <c r="C71">
-        <v>17.170000000000002</v>
+        <v>17.059999999999999</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B72" t="s">
-        <v>4</v>
+        <v>51</v>
       </c>
       <c r="C72">
-        <v>17.059999999999999</v>
+        <v>16.399999999999999</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B73" t="s">
-        <v>54</v>
+        <v>4</v>
       </c>
       <c r="C73">
-        <v>16.399999999999999</v>
+        <v>16.309999999999999</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B74" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="C74">
-        <v>16.309999999999999</v>
+        <v>16.21</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>56</v>
+        <v>179</v>
       </c>
       <c r="B75" t="s">
         <v>25</v>
       </c>
       <c r="C75">
-        <v>16.21</v>
+        <v>16.190000000000001</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>179</v>
+        <v>163</v>
       </c>
       <c r="B78">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>180</v>
+        <v>164</v>
       </c>
       <c r="B79">
-        <v>35</v>
+        <v>37</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>181</v>
+        <v>165</v>
       </c>
       <c r="B80">
         <v>68</v>

</xml_diff>

<commit_message>
Final pre-selection show predictions
</commit_message>
<xml_diff>
--- a/ncaaModelOutcomes.xlsx
+++ b/ncaaModelOutcomes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/isaiahnick/Desktop/NCAAM/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9646F57E-2962-1F45-977D-D2D70063A6BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6175780F-E761-6046-88AA-8126C9EFC3B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="780" windowWidth="28940" windowHeight="19940" activeTab="6" xr2:uid="{48E97E4C-EE8F-4D4C-B07B-683BDA3BBCA7}"/>
+    <workbookView xWindow="0" yWindow="780" windowWidth="28940" windowHeight="19940" activeTab="5" xr2:uid="{48E97E4C-EE8F-4D4C-B07B-683BDA3BBCA7}"/>
   </bookViews>
   <sheets>
     <sheet name="Champions" sheetId="2" r:id="rId1"/>
@@ -530,9 +530,6 @@
     <t>UC San Diego</t>
   </si>
   <si>
-    <t>Number of teams meeting criteria: 44</t>
-  </si>
-  <si>
     <t>Texas A&amp;M Corpus Chris</t>
   </si>
   <si>
@@ -579,6 +576,9 @@
   </si>
   <si>
     <t>SIUE</t>
+  </si>
+  <si>
+    <t>Number of teams meeting criteria: 47</t>
   </si>
 </sst>
 </file>
@@ -967,7 +967,7 @@
   <dimension ref="A1:H27"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1008,7 +1008,7 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
@@ -1401,7 +1401,7 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
@@ -1900,7 +1900,7 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
@@ -2764,7 +2764,7 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
@@ -3835,7 +3835,7 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
@@ -4839,7 +4839,7 @@
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B49" t="s">
         <v>47</v>
@@ -4865,7 +4865,7 @@
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B50" t="s">
         <v>25</v>
@@ -4949,8 +4949,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{645CF770-8328-7447-B6BD-A2D494CAA547}">
   <dimension ref="A1:H64"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4990,7 +4990,7 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>162</v>
+        <v>178</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
@@ -6040,7 +6040,7 @@
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B51" t="s">
         <v>4</v>
@@ -6066,7 +6066,7 @@
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B52" t="s">
         <v>47</v>
@@ -6144,7 +6144,7 @@
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B55" t="s">
         <v>25</v>
@@ -6170,7 +6170,7 @@
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B56" t="s">
         <v>23</v>
@@ -6280,8 +6280,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A04F142-2826-6D40-AD77-493323D02C9D}">
   <dimension ref="A1:D78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="C36" sqref="C36:C73"/>
+    <sheetView topLeftCell="A22" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="E36" sqref="E36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6428,7 +6428,7 @@
         <v>128</v>
       </c>
       <c r="C14" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D14">
         <v>13.69</v>
@@ -6527,7 +6527,7 @@
         <v>126</v>
       </c>
       <c r="C23" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D23">
         <v>4.93</v>
@@ -6549,7 +6549,7 @@
         <v>135</v>
       </c>
       <c r="C25" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D25">
         <v>2.08</v>
@@ -6571,7 +6571,7 @@
         <v>134</v>
       </c>
       <c r="C27" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D27">
         <v>0.25</v>
@@ -6604,7 +6604,7 @@
         <v>138</v>
       </c>
       <c r="C30" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D30">
         <v>-2.15</v>
@@ -6615,7 +6615,7 @@
         <v>127</v>
       </c>
       <c r="C31" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D31">
         <v>-4.3099999999999996</v>
@@ -6626,7 +6626,7 @@
         <v>141</v>
       </c>
       <c r="C32" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D32">
         <v>-4.8899999999999997</v>
@@ -7005,7 +7005,7 @@
         <v>4</v>
       </c>
       <c r="B68" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C68">
         <v>17.690000000000001</v>
@@ -7016,7 +7016,7 @@
         <v>47</v>
       </c>
       <c r="B69" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C69">
         <v>17.3</v>
@@ -7027,7 +7027,7 @@
         <v>25</v>
       </c>
       <c r="B70" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C70">
         <v>17.170000000000002</v>
@@ -7049,7 +7049,7 @@
         <v>23</v>
       </c>
       <c r="B72" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C72">
         <v>16.440000000000001</v>

</xml_diff>